<commit_message>
📊 Atualiza Excel com colunas v5: data_prevista, progresso, peso
</commit_message>
<xml_diff>
--- a/atividades_pmo.xlsx
+++ b/atividades_pmo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomaz\Documents\dashboard_pmo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CD70B0-A93D-4BF0-AA95-F0394D34900B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ABE1ED-68C6-4974-965F-BDEC8FCB73E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7CFEA5B0-84C7-4540-BF00-3AA590A6AF17}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Atividades" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Atividades!$A$1:$H$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Atividades!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="131">
   <si>
     <t>Observações</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>3.17</t>
+  </si>
+  <si>
+    <t>data_prevista</t>
   </si>
 </sst>
 </file>
@@ -470,11 +473,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,26 +813,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3C4F60-BF76-45B0-BD8E-5A967A89D04E}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="E42" sqref="E42:E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="62" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="5.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="166.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="9" max="9" width="154.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -845,16 +848,19 @@
         <v>87</v>
       </c>
       <c r="F1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -870,18 +876,21 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
+        <v>45800</v>
+      </c>
+      <c r="G2">
         <v>100</v>
       </c>
-      <c r="G2">
-        <f>F2/100</f>
+      <c r="H2">
+        <f>G2/100</f>
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -897,18 +906,21 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
+        <v>45800</v>
+      </c>
+      <c r="G3">
         <v>100</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G39" si="0">F3/100</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H39" si="0">G3/100</f>
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -924,18 +936,21 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
+        <v>45800</v>
+      </c>
+      <c r="G4">
         <v>100</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -951,18 +966,21 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
+        <v>45804</v>
+      </c>
+      <c r="G5">
         <v>80</v>
       </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G12" si="1">F5/100</f>
+      <c r="H5">
+        <f t="shared" ref="H5:H12" si="1">G5/100</f>
         <v>0.8</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -978,18 +996,21 @@
       <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
+        <v>45804</v>
+      </c>
+      <c r="G6">
         <v>80</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1005,18 +1026,21 @@
       <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
+        <v>45804</v>
+      </c>
+      <c r="G7">
         <v>80</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1032,18 +1056,21 @@
       <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
+        <v>45804</v>
+      </c>
+      <c r="G8">
         <v>80</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1059,18 +1086,21 @@
       <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
+        <v>45804</v>
+      </c>
+      <c r="G9">
         <v>80</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1086,18 +1116,21 @@
       <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
+        <v>45804</v>
+      </c>
+      <c r="G10">
         <v>80</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1113,18 +1146,21 @@
       <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
+        <v>45804</v>
+      </c>
+      <c r="G11">
         <v>80</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1140,18 +1176,21 @@
       <c r="E12" t="s">
         <v>15</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
+        <v>45804</v>
+      </c>
+      <c r="G12">
         <v>80</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1167,18 +1206,21 @@
       <c r="E13" t="s">
         <v>15</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
+        <v>45800</v>
+      </c>
+      <c r="G13">
         <v>100</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1194,18 +1236,21 @@
       <c r="E14" t="s">
         <v>15</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
+        <v>45804</v>
+      </c>
+      <c r="G14">
         <v>80</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1221,18 +1266,21 @@
       <c r="E15" t="s">
         <v>5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
+        <v>45804</v>
+      </c>
+      <c r="G15">
         <v>50</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1248,18 +1296,21 @@
       <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="F16">
-        <v>0</v>
+      <c r="F16" s="2">
+        <v>45804</v>
       </c>
       <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1275,18 +1326,21 @@
       <c r="E17" t="s">
         <v>103</v>
       </c>
-      <c r="F17">
-        <v>0</v>
+      <c r="F17" s="2">
+        <v>45804</v>
       </c>
       <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1302,18 +1356,21 @@
       <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="F18">
-        <v>0</v>
+      <c r="F18" s="2">
+        <v>45814</v>
       </c>
       <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1329,18 +1386,21 @@
       <c r="E19" t="s">
         <v>5</v>
       </c>
-      <c r="F19">
-        <v>0</v>
+      <c r="F19" s="2">
+        <v>45807</v>
       </c>
       <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1356,18 +1416,21 @@
       <c r="E20" t="s">
         <v>5</v>
       </c>
-      <c r="F20">
-        <v>0</v>
+      <c r="F20" s="2">
+        <v>45807</v>
       </c>
       <c r="G20">
-        <f t="shared" ref="G20:G32" si="2">F20/100</f>
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:H32" si="2">G20/100</f>
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -1383,18 +1446,21 @@
       <c r="E21" t="s">
         <v>5</v>
       </c>
-      <c r="F21">
-        <v>0</v>
+      <c r="F21" s="2">
+        <v>45814</v>
       </c>
       <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>122</v>
       </c>
@@ -1410,18 +1476,21 @@
       <c r="E22" t="s">
         <v>5</v>
       </c>
-      <c r="F22">
-        <v>0</v>
+      <c r="F22" s="2">
+        <v>45814</v>
       </c>
       <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>123</v>
       </c>
@@ -1437,18 +1506,21 @@
       <c r="E23" t="s">
         <v>5</v>
       </c>
-      <c r="F23">
-        <v>0</v>
+      <c r="F23" s="2">
+        <v>45814</v>
       </c>
       <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>124</v>
       </c>
@@ -1464,18 +1536,21 @@
       <c r="E24" t="s">
         <v>5</v>
       </c>
-      <c r="F24">
-        <v>0</v>
+      <c r="F24" s="2">
+        <v>45814</v>
       </c>
       <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>125</v>
       </c>
@@ -1491,18 +1566,21 @@
       <c r="E25" t="s">
         <v>5</v>
       </c>
-      <c r="F25">
-        <v>0</v>
+      <c r="F25" s="2">
+        <v>45814</v>
       </c>
       <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>126</v>
       </c>
@@ -1518,18 +1596,21 @@
       <c r="E26" t="s">
         <v>5</v>
       </c>
-      <c r="F26">
-        <v>0</v>
+      <c r="F26" s="2">
+        <v>45814</v>
       </c>
       <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>127</v>
       </c>
@@ -1545,15 +1626,18 @@
       <c r="E27" t="s">
         <v>5</v>
       </c>
-      <c r="F27">
-        <v>0</v>
+      <c r="F27" s="2">
+        <v>45814</v>
       </c>
       <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>128</v>
       </c>
@@ -1569,18 +1653,21 @@
       <c r="E28" t="s">
         <v>5</v>
       </c>
-      <c r="F28">
-        <v>0</v>
+      <c r="F28" s="2">
+        <v>45814</v>
       </c>
       <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>129</v>
       </c>
@@ -1596,18 +1683,21 @@
       <c r="E29" t="s">
         <v>5</v>
       </c>
-      <c r="F29">
-        <v>0</v>
+      <c r="F29" s="2">
+        <v>45814</v>
       </c>
       <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1623,18 +1713,21 @@
       <c r="E30" t="s">
         <v>5</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
+        <v>45800</v>
+      </c>
+      <c r="G30">
         <v>100</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1650,18 +1743,21 @@
       <c r="E31" t="s">
         <v>5</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
+        <v>45800</v>
+      </c>
+      <c r="G31">
         <v>100</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -1677,18 +1773,21 @@
       <c r="E32" t="s">
         <v>5</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
+        <v>45805</v>
+      </c>
+      <c r="G32">
         <v>75</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -1704,18 +1803,21 @@
       <c r="E33" t="s">
         <v>5</v>
       </c>
-      <c r="F33">
-        <v>100</v>
+      <c r="F33" s="2">
+        <v>45821</v>
       </c>
       <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H33" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -1731,18 +1833,21 @@
       <c r="E34" t="s">
         <v>5</v>
       </c>
-      <c r="F34">
-        <v>100</v>
+      <c r="F34" s="2">
+        <v>45821</v>
       </c>
       <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -1758,18 +1863,21 @@
       <c r="E35" t="s">
         <v>5</v>
       </c>
-      <c r="F35">
-        <v>100</v>
+      <c r="F35" s="2">
+        <v>45821</v>
       </c>
       <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H35" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -1785,15 +1893,18 @@
       <c r="E36" t="s">
         <v>5</v>
       </c>
-      <c r="F36">
-        <v>100</v>
+      <c r="F36" s="2">
+        <v>45821</v>
       </c>
       <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -1809,15 +1920,18 @@
       <c r="E37" t="s">
         <v>5</v>
       </c>
-      <c r="F37">
-        <v>100</v>
+      <c r="F37" s="2">
+        <v>45828</v>
       </c>
       <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1833,18 +1947,21 @@
       <c r="E38" t="s">
         <v>5</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
+        <v>45821</v>
+      </c>
+      <c r="G38">
         <v>75</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -1860,25 +1977,22 @@
       <c r="E39" t="s">
         <v>5</v>
       </c>
-      <c r="F39">
-        <v>100</v>
+      <c r="F39" s="2">
+        <v>45828</v>
       </c>
       <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H39" t="s">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H39" xr:uid="{CC3C4F60-BF76-45B0-BD8E-5A967A89D04E}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Fase 3 - Implantação"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I1" xr:uid="{CC3C4F60-BF76-45B0-BD8E-5A967A89D04E}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>